<commit_message>
đổi định dạng ngày khi nhập file gvm
</commit_message>
<xml_diff>
--- a/uploads/Điền thông tin GV mời KTMT 29102024(Sheet1)1.xlsx
+++ b/uploads/Điền thông tin GV mời KTMT 29102024(Sheet1)1.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="202" uniqueCount="119">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="301" uniqueCount="95">
   <si>
     <t>STT</t>
   </si>
@@ -42,12 +42,6 @@
     <t>-</t>
   </si>
   <si>
-    <t>4,4</t>
-  </si>
-  <si>
-    <t>25/05/2016</t>
-  </si>
-  <si>
     <t>22010000163 915</t>
   </si>
   <si>
@@ -75,9 +69,6 @@
     <t>Nhân viên</t>
   </si>
   <si>
-    <t>3,0</t>
-  </si>
-  <si>
     <t>25/06/2021</t>
   </si>
   <si>
@@ -87,9 +78,6 @@
     <t>n.d.thang1987@gmail.com</t>
   </si>
   <si>
-    <t>4,0</t>
-  </si>
-  <si>
     <t>NEC Vietnam Co Ltd.</t>
   </si>
   <si>
@@ -102,9 +90,6 @@
     <t>thanhvanbkhn@gmail.com</t>
   </si>
   <si>
-    <t>3,99</t>
-  </si>
-  <si>
     <t>Ngân hàng VP Bank</t>
   </si>
   <si>
@@ -129,9 +114,6 @@
     <t>anhnguyen981102@gmail.com</t>
   </si>
   <si>
-    <t>2,34</t>
-  </si>
-  <si>
     <t>21/11/1998</t>
   </si>
   <si>
@@ -147,45 +129,12 @@
     <t>MBBank, Phúc La</t>
   </si>
   <si>
-    <t>Lê Minh Tú</t>
-  </si>
-  <si>
-    <t>minhtule0199@gmail.com</t>
-  </si>
-  <si>
-    <t>29/03/2017</t>
-  </si>
-  <si>
-    <t>MBBank, Phúc Yên</t>
-  </si>
-  <si>
-    <t>Hoàng Công Tuyên</t>
-  </si>
-  <si>
     <t>hoangcongtuyen271299@gmail.com</t>
   </si>
   <si>
     <t>29/11/2016</t>
   </si>
   <si>
-    <t>duynguyen37.khoichuyen@gmail.com</t>
-  </si>
-  <si>
-    <t>20/4/2021</t>
-  </si>
-  <si>
-    <t>19/11/1979</t>
-  </si>
-  <si>
-    <t>ngand@utt.edu.vn</t>
-  </si>
-  <si>
-    <t>26/08/2022</t>
-  </si>
-  <si>
-    <t>VCB, chi nhánh HCM</t>
-  </si>
-  <si>
     <t>Họ và tên</t>
   </si>
   <si>
@@ -234,9 +183,6 @@
     <t>Bộ môn</t>
   </si>
   <si>
-    <t>Đặng Quốc Hữu</t>
-  </si>
-  <si>
     <t>Tiến sĩ</t>
   </si>
   <si>
@@ -255,9 +201,6 @@
     <t>BIDV, chi nhánh Thăng Long</t>
   </si>
   <si>
-    <t>Nguyễn Thanh Sơn</t>
-  </si>
-  <si>
     <t>Thạc sĩ</t>
   </si>
   <si>
@@ -270,18 +213,12 @@
     <t>BIDV Chi nhánh Phúc Yên, Vĩnh Phúc</t>
   </si>
   <si>
-    <t>Nguyễn Minh Tuấn</t>
-  </si>
-  <si>
     <t>Công ty TNHH phần mềm FPT</t>
   </si>
   <si>
     <t>Tổ 2 Tân Hòa, thành phố Hòa Bình, Hòa Bình</t>
   </si>
   <si>
-    <t>Nguyễn Đức Thắng</t>
-  </si>
-  <si>
     <t>Quản lý</t>
   </si>
   <si>
@@ -291,9 +228,6 @@
     <t>Ngân hàng TMCP Kỹ thương việt nam (techcombank), chi nhánh Hoàng Quốc Việt</t>
   </si>
   <si>
-    <t>Lý Thị Thanh Vân</t>
-  </si>
-  <si>
     <t>Nữ</t>
   </si>
   <si>
@@ -303,27 +237,18 @@
     <t>Thôn Nhị Trai, Trừng Xá, Lương Tài, Bắc Ninh</t>
   </si>
   <si>
-    <t>Phan Như Minh</t>
-  </si>
-  <si>
     <t xml:space="preserve">Trường Đại học Công nghệ GTVT </t>
   </si>
   <si>
     <t>TDP Tân Tiến, Tích Sơn, Thành phố Vĩnh Yên, Vĩnh Phúc</t>
   </si>
   <si>
-    <t>Phùng Văn Thuần</t>
-  </si>
-  <si>
     <t>216 B2TT GVĐH CN TVTV, Thanh Xuân Nam, T/Xuân, Hà Nội</t>
   </si>
   <si>
     <t xml:space="preserve">Ngân hàng Quốc tế VIB – chi nhánh Hai Bà Trưng </t>
   </si>
   <si>
-    <t>Nguyễn Hồng Anh</t>
-  </si>
-  <si>
     <t>GV thỉnh giảng</t>
   </si>
   <si>
@@ -336,46 +261,49 @@
     <t>Ngân hàng TMCP Ngoại thương Việt Nam (VCB), chi nhánh Nam Từ Liêm</t>
   </si>
   <si>
-    <t>Đỗ Công Minh</t>
-  </si>
-  <si>
     <t>Xa La, Hà Đông, Hà Nội</t>
   </si>
   <si>
     <t>Thực tập</t>
   </si>
   <si>
-    <t>Tráng Việt, Mê Linh, Hà Nội</t>
-  </si>
-  <si>
     <t>Xã Song Giang, huyện Gia Bình, tỉnh Bắc Ninh</t>
   </si>
   <si>
     <t>viecombank,Bắc Ninh</t>
   </si>
   <si>
-    <t>Nguyễn Văn Duy</t>
-  </si>
-  <si>
-    <t>Lập trình viên</t>
-  </si>
-  <si>
-    <t>Công ty Cổ phần Giải pháp Thanh toán Việt Nam (VNPAY)</t>
-  </si>
-  <si>
-    <t>phường Trường Thi, thành phố Vinh, tỉnh Nghệ An</t>
-  </si>
-  <si>
-    <t>Ngân hàng BIDV chi nhánh Thành Công, Hà Nội</t>
-  </si>
-  <si>
-    <t>Nguyễn Đình Nga</t>
-  </si>
-  <si>
-    <t>Trường Đại học Công nghệ Giao thông Vận tải</t>
-  </si>
-  <si>
-    <t>TDP Trung Quyên, Thị trấn Mỹ Lộc, Mỹ Lộc, Nam Định</t>
+    <t>Đặng Quốc Hữu nay</t>
+  </si>
+  <si>
+    <t>Nguyễn Thanh Sơn nay</t>
+  </si>
+  <si>
+    <t>Nguyễn Đức Thắng nay</t>
+  </si>
+  <si>
+    <t>Lý Thị Thanh Vân nay</t>
+  </si>
+  <si>
+    <t>Phan Như Minh nay</t>
+  </si>
+  <si>
+    <t>Phùng Văn Thuần nay</t>
+  </si>
+  <si>
+    <t>Nguyễn Hồng Anh nay</t>
+  </si>
+  <si>
+    <t>Đỗ Công Minh nay</t>
+  </si>
+  <si>
+    <t>Hoàng Công Tuyên nay</t>
+  </si>
+  <si>
+    <t>Nguyễn Minh Tuấn nay</t>
+  </si>
+  <si>
+    <t>25/5/2016</t>
   </si>
 </sst>
 </file>
@@ -1293,14 +1221,16 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:T14"/>
+  <dimension ref="A1:T11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I3" sqref="I3"/>
+      <selection activeCell="M2" sqref="M2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5"/>
   <cols>
+    <col min="12" max="12" width="38.1796875" customWidth="1"/>
+    <col min="13" max="13" width="18.1796875" customWidth="1"/>
     <col min="16" max="16" width="15" customWidth="1"/>
   </cols>
   <sheetData>
@@ -1309,61 +1239,61 @@
         <v>0</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>55</v>
+        <v>38</v>
       </c>
       <c r="C1" s="2" t="s">
-        <v>56</v>
+        <v>39</v>
       </c>
       <c r="D1" s="2" t="s">
         <v>1</v>
       </c>
       <c r="E1" s="2" t="s">
-        <v>57</v>
+        <v>40</v>
       </c>
       <c r="F1" s="2" t="s">
         <v>2</v>
       </c>
       <c r="G1" s="2" t="s">
-        <v>58</v>
+        <v>41</v>
       </c>
       <c r="H1" s="2" t="s">
-        <v>59</v>
+        <v>42</v>
       </c>
       <c r="I1" s="2" t="s">
-        <v>60</v>
+        <v>43</v>
       </c>
       <c r="J1" s="2" t="s">
-        <v>61</v>
+        <v>44</v>
       </c>
       <c r="K1" s="2" t="s">
-        <v>62</v>
+        <v>45</v>
       </c>
       <c r="L1" s="2" t="s">
-        <v>63</v>
+        <v>46</v>
       </c>
       <c r="M1" s="2" t="s">
-        <v>64</v>
+        <v>47</v>
       </c>
       <c r="N1" s="2" t="s">
-        <v>65</v>
+        <v>48</v>
       </c>
       <c r="O1" s="2" t="s">
-        <v>66</v>
+        <v>49</v>
       </c>
       <c r="P1" s="2" t="s">
-        <v>67</v>
+        <v>50</v>
       </c>
       <c r="Q1" s="2" t="s">
-        <v>68</v>
+        <v>51</v>
       </c>
       <c r="R1" s="2" t="s">
-        <v>69</v>
+        <v>52</v>
       </c>
       <c r="S1" s="3" t="s">
         <v>3</v>
       </c>
       <c r="T1" s="3" t="s">
-        <v>70</v>
+        <v>53</v>
       </c>
     </row>
     <row r="2" spans="1:20" ht="82.5">
@@ -1371,7 +1301,7 @@
         <v>1</v>
       </c>
       <c r="B2" s="5" t="s">
-        <v>71</v>
+        <v>84</v>
       </c>
       <c r="C2" s="5" t="s">
         <v>4</v>
@@ -1386,46 +1316,46 @@
         <v>5</v>
       </c>
       <c r="G2" s="5" t="s">
-        <v>72</v>
+        <v>54</v>
       </c>
       <c r="H2" s="5" t="s">
         <v>6</v>
       </c>
       <c r="I2" s="5" t="s">
-        <v>73</v>
-      </c>
-      <c r="J2" s="5" t="s">
-        <v>7</v>
+        <v>55</v>
+      </c>
+      <c r="J2" s="5">
+        <v>4.4000000000000004</v>
       </c>
       <c r="K2" s="5" t="s">
-        <v>74</v>
+        <v>56</v>
       </c>
       <c r="L2" s="5">
-        <v>35078000575</v>
-      </c>
-      <c r="M2" s="5" t="s">
-        <v>8</v>
+        <v>1235078000575</v>
+      </c>
+      <c r="M2" s="6">
+        <v>42425</v>
       </c>
       <c r="N2" s="5" t="s">
-        <v>75</v>
+        <v>57</v>
       </c>
       <c r="O2" s="5" t="s">
-        <v>76</v>
+        <v>58</v>
       </c>
       <c r="P2" s="5">
         <v>8519286066</v>
       </c>
       <c r="Q2" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="R2" s="5" t="s">
+        <v>59</v>
+      </c>
+      <c r="S2" s="8" t="s">
+        <v>8</v>
+      </c>
+      <c r="T2" s="8" t="s">
         <v>9</v>
-      </c>
-      <c r="R2" s="5" t="s">
-        <v>77</v>
-      </c>
-      <c r="S2" s="8" t="s">
-        <v>10</v>
-      </c>
-      <c r="T2" s="8" t="s">
-        <v>11</v>
       </c>
     </row>
     <row r="3" spans="1:20" ht="165">
@@ -1433,7 +1363,7 @@
         <v>2</v>
       </c>
       <c r="B3" s="5" t="s">
-        <v>78</v>
+        <v>85</v>
       </c>
       <c r="C3" s="5" t="s">
         <v>4</v>
@@ -1445,34 +1375,34 @@
         <v>912532175</v>
       </c>
       <c r="F3" s="7" t="s">
+        <v>10</v>
+      </c>
+      <c r="G3" s="5" t="s">
+        <v>60</v>
+      </c>
+      <c r="H3" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="I3" s="5" t="s">
+        <v>55</v>
+      </c>
+      <c r="J3" s="5">
+        <v>4.4000000000000004</v>
+      </c>
+      <c r="K3" s="5" t="s">
+        <v>61</v>
+      </c>
+      <c r="L3" s="5">
+        <v>1226075003834</v>
+      </c>
+      <c r="M3" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="G3" s="5" t="s">
-        <v>79</v>
-      </c>
-      <c r="H3" s="5" t="s">
-        <v>13</v>
-      </c>
-      <c r="I3" s="5" t="s">
-        <v>73</v>
-      </c>
-      <c r="J3" s="5" t="s">
-        <v>7</v>
-      </c>
-      <c r="K3" s="5" t="s">
-        <v>80</v>
-      </c>
-      <c r="L3" s="5">
-        <v>26075003834</v>
-      </c>
-      <c r="M3" s="5" t="s">
-        <v>14</v>
-      </c>
       <c r="N3" s="5" t="s">
-        <v>75</v>
+        <v>57</v>
       </c>
       <c r="O3" s="5" t="s">
-        <v>81</v>
+        <v>62</v>
       </c>
       <c r="P3" s="5">
         <v>8053747985</v>
@@ -1481,13 +1411,13 @@
         <v>42610000097218</v>
       </c>
       <c r="R3" s="5" t="s">
-        <v>82</v>
+        <v>63</v>
       </c>
       <c r="S3" s="9" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="T3" s="9" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
     </row>
     <row r="4" spans="1:20" ht="148.5">
@@ -1495,46 +1425,46 @@
         <v>3</v>
       </c>
       <c r="B4" s="5" t="s">
-        <v>83</v>
+        <v>93</v>
       </c>
       <c r="C4" s="5" t="s">
         <v>4</v>
       </c>
       <c r="D4" s="5" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="E4" s="5">
         <v>397851852</v>
       </c>
       <c r="F4" s="10" t="s">
+        <v>14</v>
+      </c>
+      <c r="G4" s="5" t="s">
+        <v>60</v>
+      </c>
+      <c r="H4" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="I4" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="J4" s="5">
+        <v>3</v>
+      </c>
+      <c r="K4" s="5" t="s">
+        <v>64</v>
+      </c>
+      <c r="L4" s="5">
+        <v>1217094007872</v>
+      </c>
+      <c r="M4" s="5" t="s">
         <v>16</v>
       </c>
-      <c r="G4" s="5" t="s">
-        <v>79</v>
-      </c>
-      <c r="H4" s="5" t="s">
-        <v>13</v>
-      </c>
-      <c r="I4" s="5" t="s">
-        <v>17</v>
-      </c>
-      <c r="J4" s="5" t="s">
-        <v>18</v>
-      </c>
-      <c r="K4" s="5" t="s">
-        <v>84</v>
-      </c>
-      <c r="L4" s="5">
-        <v>17094007872</v>
-      </c>
-      <c r="M4" s="5" t="s">
-        <v>19</v>
-      </c>
       <c r="N4" s="5" t="s">
-        <v>75</v>
+        <v>57</v>
       </c>
       <c r="O4" s="5" t="s">
-        <v>85</v>
+        <v>65</v>
       </c>
       <c r="P4" s="5">
         <v>8139038927</v>
@@ -1543,13 +1473,13 @@
         <v>19036977679015</v>
       </c>
       <c r="R4" s="5" t="s">
-        <v>20</v>
+        <v>17</v>
       </c>
       <c r="S4" s="8" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="T4" s="8" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
     </row>
     <row r="5" spans="1:20" ht="231">
@@ -1569,34 +1499,34 @@
         <v>977954458</v>
       </c>
       <c r="F5" s="10" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="G5" s="5" t="s">
-        <v>79</v>
+        <v>60</v>
       </c>
       <c r="H5" s="5" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="I5" s="5" t="s">
-        <v>87</v>
-      </c>
-      <c r="J5" s="5" t="s">
-        <v>22</v>
+        <v>66</v>
+      </c>
+      <c r="J5" s="5">
+        <v>4</v>
       </c>
       <c r="K5" s="5" t="s">
-        <v>23</v>
+        <v>19</v>
       </c>
       <c r="L5" s="5">
-        <v>37087003636</v>
+        <v>1237087003636</v>
       </c>
       <c r="M5" s="5" t="s">
-        <v>24</v>
+        <v>20</v>
       </c>
       <c r="N5" s="5" t="s">
-        <v>75</v>
+        <v>57</v>
       </c>
       <c r="O5" s="5" t="s">
-        <v>88</v>
+        <v>67</v>
       </c>
       <c r="P5" s="5">
         <v>8095590888</v>
@@ -1605,13 +1535,13 @@
         <v>11722307021010</v>
       </c>
       <c r="R5" s="5" t="s">
-        <v>89</v>
+        <v>68</v>
       </c>
       <c r="S5" s="8" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="T5" s="8" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
     </row>
     <row r="6" spans="1:20" ht="148.5">
@@ -1619,46 +1549,46 @@
         <v>5</v>
       </c>
       <c r="B6" s="5" t="s">
-        <v>90</v>
+        <v>87</v>
       </c>
       <c r="C6" s="5" t="s">
-        <v>91</v>
+        <v>69</v>
       </c>
       <c r="D6" s="5" t="s">
-        <v>25</v>
+        <v>21</v>
       </c>
       <c r="E6" s="5">
         <v>987629720</v>
       </c>
       <c r="F6" s="10" t="s">
-        <v>26</v>
+        <v>22</v>
       </c>
       <c r="G6" s="5" t="s">
-        <v>79</v>
+        <v>60</v>
       </c>
       <c r="H6" s="5" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="I6" s="5" t="s">
-        <v>92</v>
-      </c>
-      <c r="J6" s="5" t="s">
-        <v>27</v>
+        <v>70</v>
+      </c>
+      <c r="J6" s="5">
+        <v>3.99</v>
       </c>
       <c r="K6" s="5" t="s">
-        <v>28</v>
+        <v>23</v>
       </c>
       <c r="L6" s="5">
-        <v>33186014693</v>
+        <v>1233186014693</v>
       </c>
       <c r="M6" s="6">
         <v>44542</v>
       </c>
       <c r="N6" s="5" t="s">
-        <v>75</v>
+        <v>57</v>
       </c>
       <c r="O6" s="5" t="s">
-        <v>93</v>
+        <v>71</v>
       </c>
       <c r="P6" s="5">
         <v>8103250006</v>
@@ -1667,13 +1597,13 @@
         <v>260231097</v>
       </c>
       <c r="R6" s="5" t="s">
-        <v>29</v>
+        <v>24</v>
       </c>
       <c r="S6" s="8" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="T6" s="8" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
     </row>
     <row r="7" spans="1:20" ht="181.5">
@@ -1681,46 +1611,46 @@
         <v>6</v>
       </c>
       <c r="B7" s="5" t="s">
-        <v>94</v>
+        <v>88</v>
       </c>
       <c r="C7" s="5" t="s">
         <v>4</v>
       </c>
       <c r="D7" s="5" t="s">
-        <v>30</v>
+        <v>25</v>
       </c>
       <c r="E7" s="5">
         <v>912979207</v>
       </c>
       <c r="F7" s="10" t="s">
-        <v>31</v>
+        <v>26</v>
       </c>
       <c r="G7" s="5" t="s">
-        <v>79</v>
+        <v>60</v>
       </c>
       <c r="H7" s="5" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="I7" s="5" t="s">
-        <v>73</v>
-      </c>
-      <c r="J7" s="5" t="s">
-        <v>22</v>
+        <v>55</v>
+      </c>
+      <c r="J7" s="5">
+        <v>4</v>
       </c>
       <c r="K7" s="5" t="s">
-        <v>95</v>
+        <v>72</v>
       </c>
       <c r="L7" s="5">
-        <v>26078001538</v>
+        <v>1226078001538</v>
       </c>
       <c r="M7" s="6">
         <v>44473</v>
       </c>
       <c r="N7" s="5" t="s">
-        <v>75</v>
+        <v>57</v>
       </c>
       <c r="O7" s="5" t="s">
-        <v>96</v>
+        <v>73</v>
       </c>
       <c r="P7" s="5">
         <v>8072856122</v>
@@ -1729,13 +1659,13 @@
         <v>106003983584</v>
       </c>
       <c r="R7" s="5" t="s">
-        <v>32</v>
+        <v>27</v>
       </c>
       <c r="S7" s="8" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="T7" s="8" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
     </row>
     <row r="8" spans="1:20" ht="181.5">
@@ -1743,7 +1673,7 @@
         <v>7</v>
       </c>
       <c r="B8" s="5" t="s">
-        <v>97</v>
+        <v>89</v>
       </c>
       <c r="C8" s="5" t="s">
         <v>4</v>
@@ -1755,34 +1685,34 @@
         <v>989923698</v>
       </c>
       <c r="F8" s="10" t="s">
-        <v>33</v>
+        <v>28</v>
       </c>
       <c r="G8" s="5" t="s">
-        <v>79</v>
+        <v>60</v>
       </c>
       <c r="H8" s="5" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="I8" s="5" t="s">
-        <v>73</v>
-      </c>
-      <c r="J8" s="5" t="s">
-        <v>22</v>
+        <v>55</v>
+      </c>
+      <c r="J8" s="5">
+        <v>4</v>
       </c>
       <c r="K8" s="5" t="s">
-        <v>95</v>
+        <v>72</v>
       </c>
       <c r="L8" s="5">
-        <v>36089000558</v>
+        <v>1236089000558</v>
       </c>
       <c r="M8" s="6">
         <v>44870</v>
       </c>
       <c r="N8" s="5" t="s">
-        <v>75</v>
+        <v>57</v>
       </c>
       <c r="O8" s="5" t="s">
-        <v>98</v>
+        <v>74</v>
       </c>
       <c r="P8" s="5">
         <v>8319454690</v>
@@ -1791,13 +1721,13 @@
         <v>4704060067454</v>
       </c>
       <c r="R8" s="5" t="s">
-        <v>99</v>
+        <v>75</v>
       </c>
       <c r="S8" s="8" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="T8" s="8" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
     </row>
     <row r="9" spans="1:20" ht="214.5">
@@ -1805,59 +1735,59 @@
         <v>8</v>
       </c>
       <c r="B9" s="5" t="s">
-        <v>100</v>
+        <v>90</v>
       </c>
       <c r="C9" s="5" t="s">
         <v>4</v>
       </c>
       <c r="D9" s="5" t="s">
-        <v>34</v>
+        <v>29</v>
       </c>
       <c r="E9" s="5">
         <v>865256498</v>
       </c>
       <c r="F9" s="10" t="s">
-        <v>35</v>
+        <v>30</v>
       </c>
       <c r="G9" s="5" t="s">
-        <v>79</v>
+        <v>60</v>
       </c>
       <c r="H9" s="5" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="I9" s="5" t="s">
-        <v>101</v>
-      </c>
-      <c r="J9" s="5" t="s">
-        <v>36</v>
+        <v>76</v>
+      </c>
+      <c r="J9" s="5">
+        <v>2.34</v>
       </c>
       <c r="K9" s="5" t="s">
-        <v>102</v>
+        <v>77</v>
       </c>
       <c r="L9" s="5">
-        <v>1098007477</v>
+        <v>109800747712</v>
       </c>
       <c r="M9" s="6">
         <v>44903</v>
       </c>
       <c r="N9" s="5" t="s">
-        <v>75</v>
+        <v>57</v>
       </c>
       <c r="O9" s="5" t="s">
-        <v>103</v>
+        <v>78</v>
       </c>
       <c r="P9" s="5"/>
       <c r="Q9" s="5">
         <v>1029289578</v>
       </c>
       <c r="R9" s="5" t="s">
-        <v>104</v>
+        <v>79</v>
       </c>
       <c r="S9" s="8" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="T9" s="8" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
     </row>
     <row r="10" spans="1:20" ht="82.5">
@@ -1865,299 +1795,117 @@
         <v>9</v>
       </c>
       <c r="B10" s="5" t="s">
-        <v>105</v>
+        <v>91</v>
       </c>
       <c r="C10" s="5" t="s">
         <v>4</v>
       </c>
       <c r="D10" s="5" t="s">
-        <v>37</v>
+        <v>31</v>
       </c>
       <c r="E10" s="5">
         <v>868546800</v>
       </c>
       <c r="F10" s="10" t="s">
-        <v>38</v>
+        <v>32</v>
       </c>
       <c r="G10" s="5" t="s">
-        <v>79</v>
+        <v>60</v>
       </c>
       <c r="H10" s="5" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="I10" s="5" t="s">
-        <v>101</v>
-      </c>
-      <c r="J10" s="5" t="s">
-        <v>36</v>
+        <v>76</v>
+      </c>
+      <c r="J10" s="5">
+        <v>2.34</v>
       </c>
       <c r="K10" s="5" t="s">
-        <v>39</v>
+        <v>33</v>
       </c>
       <c r="L10" s="5">
-        <v>36098015186</v>
+        <v>1236098015186</v>
       </c>
       <c r="M10" s="5" t="s">
-        <v>40</v>
+        <v>34</v>
       </c>
       <c r="N10" s="5" t="s">
-        <v>75</v>
+        <v>57</v>
       </c>
       <c r="O10" s="5" t="s">
-        <v>106</v>
+        <v>80</v>
       </c>
       <c r="P10" s="5"/>
       <c r="Q10" s="5">
         <v>56003686</v>
       </c>
       <c r="R10" s="5" t="s">
-        <v>41</v>
+        <v>35</v>
       </c>
       <c r="S10" s="8" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="T10" s="8" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="11" spans="1:20" ht="148.5">
+      <c r="A11" s="4">
         <v>11</v>
       </c>
-    </row>
-    <row r="11" spans="1:20" ht="82.5">
-      <c r="A11" s="4">
-        <v>10</v>
-      </c>
       <c r="B11" s="5" t="s">
-        <v>42</v>
+        <v>92</v>
       </c>
       <c r="C11" s="5" t="s">
         <v>4</v>
       </c>
       <c r="D11" s="6">
-        <v>36171</v>
+        <v>36192</v>
       </c>
       <c r="E11" s="5">
-        <v>382894870</v>
+        <v>565646868</v>
       </c>
       <c r="F11" s="10" t="s">
-        <v>43</v>
+        <v>36</v>
       </c>
       <c r="G11" s="5" t="s">
-        <v>79</v>
+        <v>60</v>
       </c>
       <c r="H11" s="5" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="I11" s="5" t="s">
-        <v>107</v>
-      </c>
-      <c r="J11" s="5" t="s">
-        <v>36</v>
+        <v>81</v>
+      </c>
+      <c r="J11" s="5">
+        <v>2.34</v>
       </c>
       <c r="K11" s="5"/>
       <c r="L11" s="5">
-        <v>1099021255</v>
+        <v>12125903419</v>
       </c>
       <c r="M11" s="5" t="s">
-        <v>44</v>
+        <v>37</v>
       </c>
       <c r="N11" s="5" t="s">
-        <v>75</v>
+        <v>57</v>
       </c>
       <c r="O11" s="5" t="s">
-        <v>108</v>
+        <v>82</v>
       </c>
       <c r="P11" s="5"/>
       <c r="Q11" s="5">
-        <v>80886601111999</v>
+        <v>9965894442</v>
       </c>
       <c r="R11" s="5" t="s">
-        <v>45</v>
+        <v>83</v>
       </c>
       <c r="S11" s="9" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="T11" s="9" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="12" spans="1:20" ht="148.5">
-      <c r="A12" s="4">
-        <v>11</v>
-      </c>
-      <c r="B12" s="5" t="s">
-        <v>46</v>
-      </c>
-      <c r="C12" s="5" t="s">
-        <v>4</v>
-      </c>
-      <c r="D12" s="6">
-        <v>36192</v>
-      </c>
-      <c r="E12" s="5">
-        <v>565646868</v>
-      </c>
-      <c r="F12" s="10" t="s">
-        <v>47</v>
-      </c>
-      <c r="G12" s="5" t="s">
-        <v>79</v>
-      </c>
-      <c r="H12" s="5" t="s">
-        <v>13</v>
-      </c>
-      <c r="I12" s="5" t="s">
-        <v>107</v>
-      </c>
-      <c r="J12" s="5" t="s">
-        <v>36</v>
-      </c>
-      <c r="K12" s="5"/>
-      <c r="L12" s="5">
-        <v>125903419</v>
-      </c>
-      <c r="M12" s="5" t="s">
-        <v>48</v>
-      </c>
-      <c r="N12" s="5" t="s">
-        <v>75</v>
-      </c>
-      <c r="O12" s="5" t="s">
-        <v>109</v>
-      </c>
-      <c r="P12" s="5"/>
-      <c r="Q12" s="5">
-        <v>9965894442</v>
-      </c>
-      <c r="R12" s="5" t="s">
-        <v>110</v>
-      </c>
-      <c r="S12" s="9" t="s">
-        <v>10</v>
-      </c>
-      <c r="T12" s="9" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="13" spans="1:20" ht="181.5">
-      <c r="A13" s="4">
-        <v>12</v>
-      </c>
-      <c r="B13" s="5" t="s">
-        <v>111</v>
-      </c>
-      <c r="C13" s="5" t="s">
-        <v>4</v>
-      </c>
-      <c r="D13" s="6">
-        <v>35585</v>
-      </c>
-      <c r="E13" s="5">
-        <v>869345153</v>
-      </c>
-      <c r="F13" s="10" t="s">
-        <v>49</v>
-      </c>
-      <c r="G13" s="5" t="s">
-        <v>79</v>
-      </c>
-      <c r="H13" s="5" t="s">
-        <v>13</v>
-      </c>
-      <c r="I13" s="5" t="s">
-        <v>112</v>
-      </c>
-      <c r="J13" s="5" t="s">
-        <v>18</v>
-      </c>
-      <c r="K13" s="5" t="s">
-        <v>113</v>
-      </c>
-      <c r="L13" s="5">
-        <v>40097002182</v>
-      </c>
-      <c r="M13" s="5" t="s">
-        <v>50</v>
-      </c>
-      <c r="N13" s="5" t="s">
-        <v>75</v>
-      </c>
-      <c r="O13" s="5" t="s">
-        <v>114</v>
-      </c>
-      <c r="P13" s="5">
-        <v>8574959026</v>
-      </c>
-      <c r="Q13" s="5">
-        <v>2790461981</v>
-      </c>
-      <c r="R13" s="5" t="s">
-        <v>115</v>
-      </c>
-      <c r="S13" s="8" t="s">
-        <v>10</v>
-      </c>
-      <c r="T13" s="8" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="14" spans="1:20" ht="165">
-      <c r="A14" s="4">
-        <v>13</v>
-      </c>
-      <c r="B14" s="5" t="s">
-        <v>116</v>
-      </c>
-      <c r="C14" s="5" t="s">
-        <v>4</v>
-      </c>
-      <c r="D14" s="5" t="s">
-        <v>51</v>
-      </c>
-      <c r="E14" s="5">
-        <v>938666586</v>
-      </c>
-      <c r="F14" s="7" t="s">
-        <v>52</v>
-      </c>
-      <c r="G14" s="5" t="s">
-        <v>79</v>
-      </c>
-      <c r="H14" s="5" t="s">
-        <v>13</v>
-      </c>
-      <c r="I14" s="5" t="s">
-        <v>73</v>
-      </c>
-      <c r="J14" s="5">
-        <v>3.9</v>
-      </c>
-      <c r="K14" s="5" t="s">
-        <v>117</v>
-      </c>
-      <c r="L14" s="5">
-        <v>36079027696</v>
-      </c>
-      <c r="M14" s="5" t="s">
-        <v>53</v>
-      </c>
-      <c r="N14" s="5" t="s">
-        <v>75</v>
-      </c>
-      <c r="O14" s="5" t="s">
-        <v>118</v>
-      </c>
-      <c r="P14" s="5">
-        <v>308132087</v>
-      </c>
-      <c r="Q14" s="5">
-        <v>421000490697</v>
-      </c>
-      <c r="R14" s="5" t="s">
-        <v>54</v>
-      </c>
-      <c r="S14" s="8" t="s">
-        <v>10</v>
-      </c>
-      <c r="T14" s="8" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
     </row>
   </sheetData>
@@ -2169,9 +1917,7 @@
     <hyperlink ref="F8" r:id="rId5" display="mailto:thuanpv89@gmail.com"/>
     <hyperlink ref="F9" r:id="rId6" display="mailto:anhnguyen981102@gmail.com"/>
     <hyperlink ref="F10" r:id="rId7" display="mailto:docongminh8888@gmail.com"/>
-    <hyperlink ref="F11" r:id="rId8" display="mailto:minhtule0199@gmail.com"/>
-    <hyperlink ref="F12" r:id="rId9" display="mailto:hoangcongtuyen271299@gmail.com"/>
-    <hyperlink ref="F13" r:id="rId10" display="mailto:duynguyen37.khoichuyen@gmail.com"/>
+    <hyperlink ref="F11" r:id="rId8" display="mailto:hoangcongtuyen271299@gmail.com"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>